<commit_message>
fix: Update for L to T
</commit_message>
<xml_diff>
--- a/ai-agent-cpt/docs/aia_cpt_v1_toolkit.xlsx
+++ b/ai-agent-cpt/docs/aia_cpt_v1_toolkit.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pietervanschalkwyk/Library/CloudStorage/Dropbox/Consortiums/DTC/2025/AIA CPT WIP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gavingreen/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6FDC0BAF-4DBA-C64B-A7B3-13A67F3B6EEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9DAB0C1-7D76-5A42-A7EC-0A3DA4E470FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="21520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="34200" windowHeight="20340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AIA CPT" sheetId="1" r:id="rId1"/>
@@ -990,121 +990,13 @@
 - Decision reliability improvement with confidence weighting</t>
   </si>
   <si>
-    <t>All Archetypes (L1-L4)</t>
-  </si>
-  <si>
     <t>All Archetypes</t>
   </si>
   <si>
-    <t>L2+ (Critical for workflow and cognitive)</t>
-  </si>
-  <si>
     <t>Advanced Conversational, Workflow, Cognitive</t>
   </si>
   <si>
-    <t>L2+ (Procedural workflow and above)</t>
-  </si>
-  <si>
-    <t>L2+ (Enhanced for L3 cognitive)</t>
-  </si>
-  <si>
-    <t>L2+ (Critical for autonomous operation)</t>
-  </si>
-  <si>
-    <t>L3+ (Cognitive and MAGS)</t>
-  </si>
-  <si>
-    <t>L3+ (Advanced Planning), L4 (Complex MAGS)</t>
-  </si>
-  <si>
-    <t>L3+ (Adaptive Agents), L4 (Dynamic MAGS)</t>
-  </si>
-  <si>
-    <t>L1+ (Basic), L3+ (Advanced episodic)</t>
-  </si>
-  <si>
-    <t>L3+ (Cognitive autonomous agents)</t>
-  </si>
-  <si>
-    <t>L3+ (Advanced cognitive capabilities)</t>
-  </si>
-  <si>
-    <t>All Archetypes (Enhanced L3+)</t>
-  </si>
-  <si>
-    <t>L3+ (Cognitive with Advanced Memory)</t>
-  </si>
-  <si>
-    <t>L3+ (Advanced Cognitive Agents)</t>
-  </si>
-  <si>
-    <t>L2+ (Critical for workflow agents)</t>
-  </si>
-  <si>
-    <t>L2+ (Workflow and cognitive agents)</t>
-  </si>
-  <si>
-    <t>L1+ (Enhanced for L3+ cognitive)</t>
-  </si>
-  <si>
-    <t>L2+ (Tool-Using Agents), L4 (Complex Tool Ecosystems)</t>
-  </si>
-  <si>
-    <t>L3+ (Advanced Tool Integration), L4 (Enterprise MAGS)</t>
-  </si>
-  <si>
-    <t>L1+ (Critical for conversational agents)</t>
-  </si>
-  <si>
     <t>All Archetypes (Critical tasks)</t>
-  </si>
-  <si>
-    <t>L2+ (Multi-agent systems)</t>
-  </si>
-  <si>
-    <t>L2+ (Workflow agents), L4 (MAGS)</t>
-  </si>
-  <si>
-    <t>L2+ (Workflow and cognitive)</t>
-  </si>
-  <si>
-    <t>L4 (MAGS), Industrial Multi-Agent Systems</t>
-  </si>
-  <si>
-    <t>L4 (MAGS), Complex Multi-Agent Workflows</t>
-  </si>
-  <si>
-    <t>L4 (Industrial MAGS), Manufacturing Systems</t>
-  </si>
-  <si>
-    <t>L3+ (Enterprise Systems), L4 (Enterprise MAGS)</t>
-  </si>
-  <si>
-    <t>L2+ (Critical for Industrial MAGS), L4 (XMPro-style systems)</t>
-  </si>
-  <si>
-    <t>L4 (Production MAGS), Enterprise Multi-Agent Systems</t>
-  </si>
-  <si>
-    <t>All Production Deployments (L1-L4)</t>
-  </si>
-  <si>
-    <t>All Levels (Critical for anti-agent washing)</t>
-  </si>
-  <si>
-    <t>L2+ (Production systems)</t>
-  </si>
-  <si>
-    <t>All Levels (Critical L3-L4 autonomous)</t>
-  </si>
-  <si>
-    <t>L2+ (Critical for autonomous decisions)</t>
-  </si>
-  <si>
-    <t>All Production Systems (L1-L4)</t>
-  </si>
-  <si>
-    <t>L3+ (Autonomous Decision-Making), L4 (Trust-Critical MAGS)</t>
   </si>
   <si>
     <t>PK.OB</t>
@@ -1369,6 +1261,114 @@
   </si>
   <si>
     <t>June 2025</t>
+  </si>
+  <si>
+    <t>All Archetypes (T1-T4)</t>
+  </si>
+  <si>
+    <t>T2+ (Critical for workflow and cognitive)</t>
+  </si>
+  <si>
+    <t>T2+ (Procedural workflow and above)</t>
+  </si>
+  <si>
+    <t>T2+ (Enhanced for T3 cognitive)</t>
+  </si>
+  <si>
+    <t>T2+ (Critical for autonomous operation)</t>
+  </si>
+  <si>
+    <t>T3+ (Cognitive and MAGS)</t>
+  </si>
+  <si>
+    <t>T3+ (Advanced Planning), L4 (Complex MAGS)</t>
+  </si>
+  <si>
+    <t>T3+ (Adaptive Agents), T4 (Dynamic MAGS)</t>
+  </si>
+  <si>
+    <t>T1+ (Basic), T3+ (Advanced episodic)</t>
+  </si>
+  <si>
+    <t>T3+ (Cognitive autonomous agents)</t>
+  </si>
+  <si>
+    <t>T3+ (Advanced cognitive capabilities)</t>
+  </si>
+  <si>
+    <t>All Archetypes (Enhanced T3+)</t>
+  </si>
+  <si>
+    <t>T3+ (Cognitive with Advanced Memory)</t>
+  </si>
+  <si>
+    <t>T3+ (Advanced Cognitive Agents)</t>
+  </si>
+  <si>
+    <t>T2+ (Critical for workflow agents)</t>
+  </si>
+  <si>
+    <t>T2+ (Workflow and cognitive agents)</t>
+  </si>
+  <si>
+    <t>T1+ (Enhanced for T3+ cognitive)</t>
+  </si>
+  <si>
+    <t>T2+ (Tool-Using Agents), T4 (Complex Tool Ecosystems)</t>
+  </si>
+  <si>
+    <t>T3+ (Advanced Tool Integration), T4 (Enterprise MAGS)</t>
+  </si>
+  <si>
+    <t>T1+ (Critical for conversational agents)</t>
+  </si>
+  <si>
+    <t>T2+ (Multi-agent systems)</t>
+  </si>
+  <si>
+    <t>T2+ (Workflow agents), T4 (MAGS)</t>
+  </si>
+  <si>
+    <t>T2+ (Workflow and cognitive)</t>
+  </si>
+  <si>
+    <t>T4 (MAGS), Industrial Multi-Agent Systems</t>
+  </si>
+  <si>
+    <t>T4 (MAGS), Complex Multi-Agent Workflows</t>
+  </si>
+  <si>
+    <t>T4 (Industrial MAGS), Manufacturing Systems</t>
+  </si>
+  <si>
+    <t>T3+ (Enterprise Systems), T4 (Enterprise MAGS)</t>
+  </si>
+  <si>
+    <t>T2+ (Critical for Industrial MAGS), T4</t>
+  </si>
+  <si>
+    <t>T4 (Production MAGS), Enterprise Multi-Agent Systems</t>
+  </si>
+  <si>
+    <t>All Production Deployments (T1-T4)</t>
+  </si>
+  <si>
+    <t>T2+ (Production systems)</t>
+  </si>
+  <si>
+    <t>T2+ (Critical for autonomous decisions)</t>
+  </si>
+  <si>
+    <t>All Production Systems (T1-T4)</t>
+  </si>
+  <si>
+    <t>T3+ (Autonomous Decision-Making), T4 (Trust-Critical MAGS)</t>
+  </si>
+  <si>
+    <t>All Types (Critical for anti-agent washing)</t>
+  </si>
+  <si>
+    <t>All Types (Critical T3-T4 autonomous)</t>
   </si>
 </sst>
 </file>
@@ -2105,8 +2105,8 @@
   </sheetPr>
   <dimension ref="B2:I55"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -2125,19 +2125,19 @@
   <sheetData>
     <row r="2" spans="2:9" s="31" customFormat="1" ht="32">
       <c r="B2" s="30" t="s">
-        <v>355</v>
+        <v>319</v>
       </c>
       <c r="E2" s="32"/>
       <c r="F2" s="32"/>
       <c r="G2" s="32"/>
       <c r="H2" s="39" t="s">
-        <v>356</v>
+        <v>320</v>
       </c>
     </row>
     <row r="3" spans="2:9" ht="29" customHeight="1" thickBot="1"/>
     <row r="4" spans="2:9" s="25" customFormat="1" ht="23">
       <c r="B4" s="26" t="s">
-        <v>327</v>
+        <v>291</v>
       </c>
       <c r="C4" s="27" t="s">
         <v>0</v>
@@ -2163,10 +2163,10 @@
     </row>
     <row r="5" spans="2:9" s="6" customFormat="1" ht="23">
       <c r="B5" s="14" t="s">
-        <v>316</v>
+        <v>280</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>315</v>
+        <v>279</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="4"/>
@@ -2177,7 +2177,7 @@
     </row>
     <row r="6" spans="2:9" ht="68">
       <c r="B6" s="16" t="s">
-        <v>270</v>
+        <v>234</v>
       </c>
       <c r="C6" s="12"/>
       <c r="D6" s="12" t="s">
@@ -2196,12 +2196,12 @@
         <v>186</v>
       </c>
       <c r="I6" s="17" t="s">
-        <v>231</v>
+        <v>321</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="68">
       <c r="B7" s="16" t="s">
-        <v>271</v>
+        <v>235</v>
       </c>
       <c r="C7" s="12"/>
       <c r="D7" s="12" t="s">
@@ -2220,12 +2220,12 @@
         <v>187</v>
       </c>
       <c r="I7" s="17" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="68">
       <c r="B8" s="16" t="s">
-        <v>272</v>
+        <v>236</v>
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="12" t="s">
@@ -2244,12 +2244,12 @@
         <v>188</v>
       </c>
       <c r="I8" s="17" t="s">
-        <v>233</v>
+        <v>322</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="68">
       <c r="B9" s="16" t="s">
-        <v>273</v>
+        <v>237</v>
       </c>
       <c r="C9" s="12"/>
       <c r="D9" s="12" t="s">
@@ -2268,15 +2268,15 @@
         <v>189</v>
       </c>
       <c r="I9" s="17" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="10" spans="2:9" s="3" customFormat="1" ht="22">
       <c r="B10" s="18" t="s">
-        <v>318</v>
+        <v>282</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>317</v>
+        <v>281</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="10"/>
@@ -2287,7 +2287,7 @@
     </row>
     <row r="11" spans="2:9" ht="68">
       <c r="B11" s="16" t="s">
-        <v>274</v>
+        <v>238</v>
       </c>
       <c r="C11" s="12"/>
       <c r="D11" s="12" t="s">
@@ -2306,12 +2306,12 @@
         <v>190</v>
       </c>
       <c r="I11" s="17" t="s">
-        <v>235</v>
+        <v>323</v>
       </c>
     </row>
     <row r="12" spans="2:9" ht="68">
       <c r="B12" s="16" t="s">
-        <v>275</v>
+        <v>239</v>
       </c>
       <c r="C12" s="12"/>
       <c r="D12" s="12" t="s">
@@ -2330,12 +2330,12 @@
         <v>191</v>
       </c>
       <c r="I12" s="17" t="s">
-        <v>236</v>
+        <v>324</v>
       </c>
     </row>
     <row r="13" spans="2:9" ht="68">
       <c r="B13" s="16" t="s">
-        <v>276</v>
+        <v>240</v>
       </c>
       <c r="C13" s="12"/>
       <c r="D13" s="12" t="s">
@@ -2354,12 +2354,12 @@
         <v>192</v>
       </c>
       <c r="I13" s="17" t="s">
-        <v>237</v>
+        <v>325</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="68">
       <c r="B14" s="16" t="s">
-        <v>277</v>
+        <v>241</v>
       </c>
       <c r="C14" s="12"/>
       <c r="D14" s="12" t="s">
@@ -2378,12 +2378,12 @@
         <v>193</v>
       </c>
       <c r="I14" s="17" t="s">
-        <v>238</v>
+        <v>326</v>
       </c>
     </row>
     <row r="15" spans="2:9" ht="68">
       <c r="B15" s="38" t="s">
-        <v>278</v>
+        <v>242</v>
       </c>
       <c r="C15" s="12"/>
       <c r="D15" s="12" t="s">
@@ -2393,7 +2393,7 @@
         <v>60</v>
       </c>
       <c r="F15" s="33" t="s">
-        <v>328</v>
+        <v>292</v>
       </c>
       <c r="G15" s="13" t="s">
         <v>149</v>
@@ -2402,12 +2402,12 @@
         <v>194</v>
       </c>
       <c r="I15" s="17" t="s">
-        <v>239</v>
+        <v>327</v>
       </c>
     </row>
     <row r="16" spans="2:9" ht="68">
       <c r="B16" s="16" t="s">
-        <v>279</v>
+        <v>243</v>
       </c>
       <c r="C16" s="12"/>
       <c r="D16" s="12" t="s">
@@ -2426,15 +2426,15 @@
         <v>195</v>
       </c>
       <c r="I16" s="17" t="s">
-        <v>240</v>
+        <v>328</v>
       </c>
     </row>
     <row r="17" spans="2:9" s="7" customFormat="1" ht="22">
       <c r="B17" s="18" t="s">
-        <v>320</v>
+        <v>284</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>319</v>
+        <v>283</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="11"/>
@@ -2445,7 +2445,7 @@
     </row>
     <row r="18" spans="2:9" ht="68">
       <c r="B18" s="16" t="s">
-        <v>280</v>
+        <v>244</v>
       </c>
       <c r="C18" s="12"/>
       <c r="D18" s="12" t="s">
@@ -2464,12 +2464,12 @@
         <v>196</v>
       </c>
       <c r="I18" s="17" t="s">
-        <v>241</v>
+        <v>329</v>
       </c>
     </row>
     <row r="19" spans="2:9" ht="68">
       <c r="B19" s="16" t="s">
-        <v>281</v>
+        <v>245</v>
       </c>
       <c r="C19" s="12"/>
       <c r="D19" s="12" t="s">
@@ -2488,12 +2488,12 @@
         <v>197</v>
       </c>
       <c r="I19" s="17" t="s">
-        <v>242</v>
+        <v>330</v>
       </c>
     </row>
     <row r="20" spans="2:9" ht="68">
       <c r="B20" s="16" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="C20" s="12"/>
       <c r="D20" s="12" t="s">
@@ -2512,12 +2512,12 @@
         <v>198</v>
       </c>
       <c r="I20" s="17" t="s">
-        <v>243</v>
+        <v>331</v>
       </c>
     </row>
     <row r="21" spans="2:9" ht="68">
       <c r="B21" s="16" t="s">
-        <v>283</v>
+        <v>247</v>
       </c>
       <c r="C21" s="12"/>
       <c r="D21" s="12" t="s">
@@ -2536,12 +2536,12 @@
         <v>199</v>
       </c>
       <c r="I21" s="17" t="s">
-        <v>244</v>
+        <v>332</v>
       </c>
     </row>
     <row r="22" spans="2:9" ht="68">
       <c r="B22" s="16" t="s">
-        <v>284</v>
+        <v>248</v>
       </c>
       <c r="C22" s="12"/>
       <c r="D22" s="12" t="s">
@@ -2560,12 +2560,12 @@
         <v>200</v>
       </c>
       <c r="I22" s="17" t="s">
-        <v>245</v>
+        <v>333</v>
       </c>
     </row>
     <row r="23" spans="2:9" ht="68">
       <c r="B23" s="16" t="s">
-        <v>285</v>
+        <v>249</v>
       </c>
       <c r="C23" s="12"/>
       <c r="D23" s="12" t="s">
@@ -2584,15 +2584,15 @@
         <v>201</v>
       </c>
       <c r="I23" s="17" t="s">
-        <v>246</v>
+        <v>334</v>
       </c>
     </row>
     <row r="24" spans="2:9" s="3" customFormat="1" ht="22">
       <c r="B24" s="18" t="s">
-        <v>322</v>
+        <v>286</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>321</v>
+        <v>285</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="10"/>
@@ -2603,7 +2603,7 @@
     </row>
     <row r="25" spans="2:9" ht="68">
       <c r="B25" s="16" t="s">
-        <v>286</v>
+        <v>250</v>
       </c>
       <c r="C25" s="12"/>
       <c r="D25" s="12" t="s">
@@ -2622,12 +2622,12 @@
         <v>202</v>
       </c>
       <c r="I25" s="17" t="s">
-        <v>231</v>
+        <v>321</v>
       </c>
     </row>
     <row r="26" spans="2:9" ht="68">
       <c r="B26" s="16" t="s">
-        <v>287</v>
+        <v>251</v>
       </c>
       <c r="C26" s="12"/>
       <c r="D26" s="12" t="s">
@@ -2646,12 +2646,12 @@
         <v>203</v>
       </c>
       <c r="I26" s="17" t="s">
-        <v>247</v>
+        <v>335</v>
       </c>
     </row>
     <row r="27" spans="2:9" ht="68">
       <c r="B27" s="16" t="s">
-        <v>288</v>
+        <v>252</v>
       </c>
       <c r="C27" s="12"/>
       <c r="D27" s="12" t="s">
@@ -2670,12 +2670,12 @@
         <v>204</v>
       </c>
       <c r="I27" s="17" t="s">
-        <v>248</v>
+        <v>336</v>
       </c>
     </row>
     <row r="28" spans="2:9" ht="68">
       <c r="B28" s="16" t="s">
-        <v>289</v>
+        <v>253</v>
       </c>
       <c r="C28" s="12"/>
       <c r="D28" s="12" t="s">
@@ -2694,12 +2694,12 @@
         <v>205</v>
       </c>
       <c r="I28" s="17" t="s">
-        <v>249</v>
+        <v>337</v>
       </c>
     </row>
     <row r="29" spans="2:9" ht="68">
       <c r="B29" s="16" t="s">
-        <v>290</v>
+        <v>254</v>
       </c>
       <c r="C29" s="12"/>
       <c r="D29" s="12" t="s">
@@ -2718,12 +2718,12 @@
         <v>206</v>
       </c>
       <c r="I29" s="17" t="s">
-        <v>250</v>
+        <v>338</v>
       </c>
     </row>
     <row r="30" spans="2:9" ht="68">
       <c r="B30" s="16" t="s">
-        <v>291</v>
+        <v>255</v>
       </c>
       <c r="C30" s="12"/>
       <c r="D30" s="12" t="s">
@@ -2742,15 +2742,15 @@
         <v>207</v>
       </c>
       <c r="I30" s="17" t="s">
-        <v>251</v>
+        <v>339</v>
       </c>
     </row>
     <row r="31" spans="2:9" s="7" customFormat="1" ht="22">
       <c r="B31" s="18" t="s">
-        <v>324</v>
+        <v>288</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>323</v>
+        <v>287</v>
       </c>
       <c r="D31" s="8"/>
       <c r="E31" s="11"/>
@@ -2761,7 +2761,7 @@
     </row>
     <row r="32" spans="2:9" ht="68">
       <c r="B32" s="16" t="s">
-        <v>292</v>
+        <v>256</v>
       </c>
       <c r="C32" s="12"/>
       <c r="D32" s="12" t="s">
@@ -2780,12 +2780,12 @@
         <v>208</v>
       </c>
       <c r="I32" s="17" t="s">
-        <v>231</v>
+        <v>321</v>
       </c>
     </row>
     <row r="33" spans="2:9" ht="68">
       <c r="B33" s="16" t="s">
-        <v>293</v>
+        <v>257</v>
       </c>
       <c r="C33" s="12"/>
       <c r="D33" s="12" t="s">
@@ -2804,12 +2804,12 @@
         <v>209</v>
       </c>
       <c r="I33" s="17" t="s">
-        <v>252</v>
+        <v>340</v>
       </c>
     </row>
     <row r="34" spans="2:9" ht="68">
       <c r="B34" s="16" t="s">
-        <v>294</v>
+        <v>258</v>
       </c>
       <c r="C34" s="12"/>
       <c r="D34" s="12" t="s">
@@ -2828,12 +2828,12 @@
         <v>210</v>
       </c>
       <c r="I34" s="17" t="s">
-        <v>253</v>
+        <v>233</v>
       </c>
     </row>
     <row r="35" spans="2:9" ht="68">
       <c r="B35" s="16" t="s">
-        <v>295</v>
+        <v>259</v>
       </c>
       <c r="C35" s="12"/>
       <c r="D35" s="12" t="s">
@@ -2852,12 +2852,12 @@
         <v>211</v>
       </c>
       <c r="I35" s="17" t="s">
-        <v>254</v>
+        <v>341</v>
       </c>
     </row>
     <row r="36" spans="2:9" ht="68">
       <c r="B36" s="16" t="s">
-        <v>296</v>
+        <v>260</v>
       </c>
       <c r="C36" s="12"/>
       <c r="D36" s="12" t="s">
@@ -2876,12 +2876,12 @@
         <v>212</v>
       </c>
       <c r="I36" s="17" t="s">
-        <v>255</v>
+        <v>342</v>
       </c>
     </row>
     <row r="37" spans="2:9" ht="68">
       <c r="B37" s="16" t="s">
-        <v>297</v>
+        <v>261</v>
       </c>
       <c r="C37" s="12"/>
       <c r="D37" s="12" t="s">
@@ -2900,12 +2900,12 @@
         <v>213</v>
       </c>
       <c r="I37" s="17" t="s">
-        <v>256</v>
+        <v>343</v>
       </c>
     </row>
     <row r="38" spans="2:9" ht="68">
       <c r="B38" s="16" t="s">
-        <v>298</v>
+        <v>262</v>
       </c>
       <c r="C38" s="12"/>
       <c r="D38" s="12" t="s">
@@ -2924,12 +2924,12 @@
         <v>214</v>
       </c>
       <c r="I38" s="17" t="s">
-        <v>257</v>
+        <v>344</v>
       </c>
     </row>
     <row r="39" spans="2:9" ht="68">
       <c r="B39" s="16" t="s">
-        <v>299</v>
+        <v>263</v>
       </c>
       <c r="C39" s="12"/>
       <c r="D39" s="12" t="s">
@@ -2948,12 +2948,12 @@
         <v>215</v>
       </c>
       <c r="I39" s="17" t="s">
-        <v>258</v>
+        <v>345</v>
       </c>
     </row>
     <row r="40" spans="2:9" ht="68">
       <c r="B40" s="16" t="s">
-        <v>300</v>
+        <v>264</v>
       </c>
       <c r="C40" s="12"/>
       <c r="D40" s="12" t="s">
@@ -2972,12 +2972,12 @@
         <v>216</v>
       </c>
       <c r="I40" s="17" t="s">
-        <v>259</v>
+        <v>346</v>
       </c>
     </row>
     <row r="41" spans="2:9" ht="68">
       <c r="B41" s="16" t="s">
-        <v>301</v>
+        <v>265</v>
       </c>
       <c r="C41" s="12"/>
       <c r="D41" s="12" t="s">
@@ -2996,12 +2996,12 @@
         <v>217</v>
       </c>
       <c r="I41" s="17" t="s">
-        <v>260</v>
+        <v>347</v>
       </c>
     </row>
     <row r="42" spans="2:9" ht="85">
       <c r="B42" s="16" t="s">
-        <v>302</v>
+        <v>266</v>
       </c>
       <c r="C42" s="12"/>
       <c r="D42" s="12" t="s">
@@ -3020,12 +3020,12 @@
         <v>218</v>
       </c>
       <c r="I42" s="17" t="s">
-        <v>261</v>
+        <v>348</v>
       </c>
     </row>
     <row r="43" spans="2:9" ht="85">
       <c r="B43" s="16" t="s">
-        <v>303</v>
+        <v>267</v>
       </c>
       <c r="C43" s="12"/>
       <c r="D43" s="12" t="s">
@@ -3044,15 +3044,15 @@
         <v>219</v>
       </c>
       <c r="I43" s="17" t="s">
-        <v>262</v>
+        <v>349</v>
       </c>
     </row>
     <row r="44" spans="2:9" s="7" customFormat="1" ht="22">
       <c r="B44" s="18" t="s">
-        <v>326</v>
+        <v>290</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>325</v>
+        <v>289</v>
       </c>
       <c r="D44" s="8"/>
       <c r="E44" s="11"/>
@@ -3063,7 +3063,7 @@
     </row>
     <row r="45" spans="2:9" ht="68">
       <c r="B45" s="16" t="s">
-        <v>304</v>
+        <v>268</v>
       </c>
       <c r="C45" s="12"/>
       <c r="D45" s="12" t="s">
@@ -3082,12 +3082,12 @@
         <v>220</v>
       </c>
       <c r="I45" s="17" t="s">
-        <v>263</v>
+        <v>350</v>
       </c>
     </row>
     <row r="46" spans="2:9" ht="68">
       <c r="B46" s="16" t="s">
-        <v>305</v>
+        <v>269</v>
       </c>
       <c r="C46" s="12"/>
       <c r="D46" s="12" t="s">
@@ -3106,12 +3106,12 @@
         <v>221</v>
       </c>
       <c r="I46" s="17" t="s">
-        <v>263</v>
+        <v>350</v>
       </c>
     </row>
     <row r="47" spans="2:9" ht="68">
       <c r="B47" s="16" t="s">
-        <v>306</v>
+        <v>270</v>
       </c>
       <c r="C47" s="12"/>
       <c r="D47" s="12" t="s">
@@ -3130,12 +3130,12 @@
         <v>222</v>
       </c>
       <c r="I47" s="17" t="s">
-        <v>264</v>
+        <v>355</v>
       </c>
     </row>
     <row r="48" spans="2:9" ht="68">
       <c r="B48" s="16" t="s">
-        <v>307</v>
+        <v>271</v>
       </c>
       <c r="C48" s="12"/>
       <c r="D48" s="12" t="s">
@@ -3154,12 +3154,12 @@
         <v>223</v>
       </c>
       <c r="I48" s="17" t="s">
-        <v>265</v>
+        <v>351</v>
       </c>
     </row>
     <row r="49" spans="2:9" ht="68">
       <c r="B49" s="16" t="s">
-        <v>308</v>
+        <v>272</v>
       </c>
       <c r="C49" s="12"/>
       <c r="D49" s="12" t="s">
@@ -3178,12 +3178,12 @@
         <v>224</v>
       </c>
       <c r="I49" s="17" t="s">
-        <v>266</v>
+        <v>356</v>
       </c>
     </row>
     <row r="50" spans="2:9" ht="68">
       <c r="B50" s="16" t="s">
-        <v>309</v>
+        <v>273</v>
       </c>
       <c r="C50" s="12"/>
       <c r="D50" s="12" t="s">
@@ -3202,12 +3202,12 @@
         <v>225</v>
       </c>
       <c r="I50" s="17" t="s">
-        <v>231</v>
+        <v>321</v>
       </c>
     </row>
     <row r="51" spans="2:9" ht="68">
       <c r="B51" s="16" t="s">
-        <v>310</v>
+        <v>274</v>
       </c>
       <c r="C51" s="12"/>
       <c r="D51" s="12" t="s">
@@ -3226,12 +3226,12 @@
         <v>226</v>
       </c>
       <c r="I51" s="17" t="s">
-        <v>267</v>
+        <v>352</v>
       </c>
     </row>
     <row r="52" spans="2:9" ht="68">
       <c r="B52" s="16" t="s">
-        <v>311</v>
+        <v>275</v>
       </c>
       <c r="C52" s="12"/>
       <c r="D52" s="12" t="s">
@@ -3250,12 +3250,12 @@
         <v>227</v>
       </c>
       <c r="I52" s="17" t="s">
-        <v>268</v>
+        <v>353</v>
       </c>
     </row>
     <row r="53" spans="2:9" ht="68">
       <c r="B53" s="16" t="s">
-        <v>312</v>
+        <v>276</v>
       </c>
       <c r="C53" s="12"/>
       <c r="D53" s="12" t="s">
@@ -3274,12 +3274,12 @@
         <v>228</v>
       </c>
       <c r="I53" s="17" t="s">
-        <v>244</v>
+        <v>332</v>
       </c>
     </row>
     <row r="54" spans="2:9" ht="68">
       <c r="B54" s="16" t="s">
-        <v>313</v>
+        <v>277</v>
       </c>
       <c r="C54" s="12"/>
       <c r="D54" s="12" t="s">
@@ -3298,12 +3298,12 @@
         <v>229</v>
       </c>
       <c r="I54" s="17" t="s">
-        <v>231</v>
+        <v>321</v>
       </c>
     </row>
     <row r="55" spans="2:9" ht="69" thickBot="1">
       <c r="B55" s="21" t="s">
-        <v>314</v>
+        <v>278</v>
       </c>
       <c r="C55" s="22"/>
       <c r="D55" s="22" t="s">
@@ -3322,7 +3322,7 @@
         <v>230</v>
       </c>
       <c r="I55" s="24" t="s">
-        <v>269</v>
+        <v>354</v>
       </c>
     </row>
   </sheetData>
@@ -3333,7 +3333,6 @@
   <pageSetup paperSize="9" scale="23" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <headerFooter>
     <oddHeader>&amp;R&amp;"Calibri,Regular"&amp;K000000Draft AI Agent Capabilities Periodic Table</oddHeader>
-    <oddFooter>&amp;L&amp;"Calibri,Regular"&amp;K000000Copyright ©️ XMPro Inc 2025</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -3356,106 +3355,106 @@
   <sheetData>
     <row r="2" spans="1:2" ht="17">
       <c r="A2" s="37" t="s">
-        <v>329</v>
+        <v>293</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>330</v>
+        <v>294</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17">
       <c r="A3" s="34" t="s">
-        <v>331</v>
+        <v>295</v>
       </c>
       <c r="B3" s="36" t="s">
-        <v>332</v>
+        <v>296</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17">
       <c r="A4" s="34" t="s">
-        <v>333</v>
+        <v>297</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>334</v>
+        <v>298</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17">
       <c r="A5" s="34" t="s">
-        <v>335</v>
+        <v>299</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>336</v>
+        <v>300</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="17">
       <c r="A6" s="34" t="s">
-        <v>337</v>
+        <v>301</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>338</v>
+        <v>302</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="17">
       <c r="A7" s="34" t="s">
-        <v>339</v>
+        <v>303</v>
       </c>
       <c r="B7" s="36" t="s">
-        <v>340</v>
+        <v>304</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="17">
       <c r="A8" s="34" t="s">
-        <v>341</v>
+        <v>305</v>
       </c>
       <c r="B8" s="36" t="s">
-        <v>342</v>
+        <v>306</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="17">
       <c r="A9" s="34" t="s">
-        <v>343</v>
+        <v>307</v>
       </c>
       <c r="B9" s="36" t="s">
-        <v>344</v>
+        <v>308</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="17">
       <c r="A10" s="34" t="s">
-        <v>345</v>
+        <v>309</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>346</v>
+        <v>310</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="17">
       <c r="A11" s="34" t="s">
-        <v>347</v>
+        <v>311</v>
       </c>
       <c r="B11" s="36" t="s">
-        <v>348</v>
+        <v>312</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="17">
       <c r="A12" s="34" t="s">
-        <v>349</v>
+        <v>313</v>
       </c>
       <c r="B12" s="36" t="s">
-        <v>350</v>
+        <v>314</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="17">
       <c r="A13" s="34" t="s">
-        <v>351</v>
+        <v>315</v>
       </c>
       <c r="B13" s="36" t="s">
-        <v>352</v>
+        <v>316</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="17">
       <c r="A14" s="34" t="s">
-        <v>353</v>
+        <v>317</v>
       </c>
       <c r="B14" s="36" t="s">
-        <v>354</v>
+        <v>318</v>
       </c>
     </row>
   </sheetData>
@@ -3706,15 +3705,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="7c7238bb-4fa8-4cb8-aec0-ea00a47779f1" xsi:nil="true"/>
@@ -3723,6 +3713,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3745,14 +3744,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC1E6ADE-8D33-4A1B-8720-B60A2432C5F4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5E5D867-88D4-4558-B737-89ACEA126000}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -3769,6 +3760,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC1E6ADE-8D33-4A1B-8720-B60A2432C5F4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{7183695d-bb12-4ebf-8539-e422da05c75a}" enabled="1" method="Standard" siteId="{67d61595-6249-4ce8-b75a-a4389468f5c6}" removed="0"/>

</xml_diff>